<commit_message>
delete cascade implemented and view bugs fixed
</commit_message>
<xml_diff>
--- a/Problems to be solved.xlsx
+++ b/Problems to be solved.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="43">
   <si>
     <t>Category</t>
   </si>
@@ -354,7 +354,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -381,8 +381,8 @@
   </sheetPr>
   <dimension ref="A1:D39"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A18" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B21" activeCellId="0" sqref="B21"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A21" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C35" activeCellId="0" sqref="C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -467,7 +467,9 @@
       <c r="B8" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="15"/>
+      <c r="C8" s="15" t="s">
+        <v>6</v>
+      </c>
       <c r="D8" s="14"/>
     </row>
     <row r="9" s="12" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -503,7 +505,9 @@
       <c r="B12" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="C12" s="16"/>
+      <c r="C12" s="16" t="s">
+        <v>6</v>
+      </c>
       <c r="D12" s="14"/>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -653,7 +657,9 @@
       <c r="B30" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="C30" s="15"/>
+      <c r="C30" s="15" t="s">
+        <v>6</v>
+      </c>
       <c r="D30" s="14"/>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -661,7 +667,9 @@
       <c r="B31" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="C31" s="15"/>
+      <c r="C31" s="15" t="s">
+        <v>6</v>
+      </c>
       <c r="D31" s="14"/>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -669,7 +677,9 @@
       <c r="B32" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="C32" s="15"/>
+      <c r="C32" s="15" t="s">
+        <v>6</v>
+      </c>
       <c r="D32" s="14"/>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -677,7 +687,9 @@
       <c r="B33" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="C33" s="15"/>
+      <c r="C33" s="15" t="s">
+        <v>6</v>
+      </c>
       <c r="D33" s="14"/>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -685,7 +697,9 @@
       <c r="B34" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="C34" s="15"/>
+      <c r="C34" s="15" t="s">
+        <v>6</v>
+      </c>
       <c r="D34" s="14"/>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -693,7 +707,9 @@
       <c r="B35" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="C35" s="15"/>
+      <c r="C35" s="15" t="s">
+        <v>6</v>
+      </c>
       <c r="D35" s="14"/>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -709,7 +725,9 @@
       <c r="B37" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="C37" s="15"/>
+      <c r="C37" s="15" t="s">
+        <v>6</v>
+      </c>
       <c r="D37" s="14"/>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -717,7 +735,9 @@
       <c r="B38" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="C38" s="15"/>
+      <c r="C38" s="15" t="s">
+        <v>6</v>
+      </c>
       <c r="D38" s="14"/>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>